<commit_message>
Prepare series_data with latest_year_value
</commit_message>
<xml_diff>
--- a/master_data/MINSET_Indicators.xlsx
+++ b/master_data/MINSET_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\ARCGIS HUBS\gender_data_portal\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B904781-9861-4577-B66B-279E12931E98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AF03D3-0C45-427B-9F4E-786393095A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1381B5DD-575F-4471-A56A-01C3E7D6FF5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{1381B5DD-575F-4471-A56A-01C3E7D6FF5C}"/>
   </bookViews>
   <sheets>
     <sheet name="CL_INDICATORS" sheetId="1" r:id="rId1"/>
@@ -672,13 +672,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="10"/>
-      <name val="MS Sans Serif"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
     </font>
@@ -703,35 +698,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,2341 +1169,2326 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FCF6FD-9172-451A-980F-6EB0E80E8E38}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="25.7109375" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="25.5">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="8">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8">
-        <v>2</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3">
         <v>14</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="8">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="9">
-        <v>2</v>
-      </c>
-      <c r="M4" s="8" t="s">
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="89.25">
-      <c r="A5" s="8">
+    <row r="5" spans="1:15">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5">
         <v>15</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="9">
-        <v>2</v>
-      </c>
-      <c r="M5" s="8" t="s">
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="89.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:15">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="9">
-        <v>2</v>
-      </c>
-      <c r="M6" s="8" t="s">
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="89.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:15">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7">
         <v>14</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="9">
-        <v>2</v>
-      </c>
-      <c r="M7" s="8" t="s">
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="8">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8">
         <v>13</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="9">
-        <v>2</v>
-      </c>
-      <c r="M8" s="8" t="s">
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="89.25">
-      <c r="A9" s="8">
+    <row r="9" spans="1:15">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>1</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9">
         <v>9</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="9">
-        <v>2</v>
-      </c>
-      <c r="M9" s="8" t="s">
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="8">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>2</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="9">
-        <v>2</v>
-      </c>
-      <c r="M10" s="8" t="s">
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
         <v>27</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="8">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11">
         <v>10</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="9">
-        <v>2</v>
-      </c>
-      <c r="M11" s="8" t="s">
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
         <v>27</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="8">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12">
         <v>16</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12">
         <v>12</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" t="s">
         <v>52</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="8">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
-        <v>2</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13">
         <v>17</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" t="s">
         <v>56</v>
       </c>
-      <c r="L13" s="9">
-        <v>1</v>
-      </c>
-      <c r="M13" s="8" t="s">
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
         <v>57</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" t="s">
         <v>58</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="102">
-      <c r="A14" s="8">
+    <row r="14" spans="1:15">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="8">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <v>2</v>
-      </c>
-      <c r="F14" s="8">
-        <v>1</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" t="s">
         <v>61</v>
       </c>
-      <c r="L14" s="9">
-        <v>2</v>
-      </c>
-      <c r="M14" s="8" t="s">
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
         <v>27</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="N14" t="s">
         <v>62</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="8">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="8">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
-        <v>2</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" t="s">
         <v>65</v>
       </c>
-      <c r="L15" s="9">
-        <v>2</v>
-      </c>
-      <c r="M15" s="8" t="s">
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="8">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="F16" s="8">
-        <v>1</v>
-      </c>
-      <c r="G16" s="8" t="s">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" t="s">
         <v>67</v>
       </c>
-      <c r="L16" s="9">
-        <v>2</v>
-      </c>
-      <c r="M16" s="8" t="s">
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="8">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>3</v>
       </c>
-      <c r="F17" s="8">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" t="s">
         <v>67</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17">
         <v>5</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="25.5">
-      <c r="A18" s="8">
+    <row r="18" spans="1:15">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="8">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>1</v>
-      </c>
-      <c r="F18" s="8">
-        <v>1</v>
-      </c>
-      <c r="G18" s="8" t="s">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" t="s">
         <v>72</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18">
         <v>4</v>
       </c>
-      <c r="M18" s="8" t="s">
+      <c r="M18" t="s">
         <v>73</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="N18" t="s">
         <v>74</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O18" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="8">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <v>2</v>
-      </c>
-      <c r="F19" s="8">
-        <v>1</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" t="s">
         <v>71</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" t="s">
         <v>72</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19">
         <v>4</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="M19" t="s">
         <v>73</v>
       </c>
-      <c r="N19" s="8" t="s">
+      <c r="N19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="8">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>3</v>
       </c>
-      <c r="F20" s="8">
-        <v>1</v>
-      </c>
-      <c r="G20" s="8" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" t="s">
         <v>71</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20">
         <v>4</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="M20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="8">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
-        <v>2</v>
-      </c>
-      <c r="G21" s="8" t="s">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
         <v>80</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" t="s">
         <v>81</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" t="s">
         <v>82</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21">
         <v>6</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="M21" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="8">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-      <c r="E22" s="8">
-        <v>1</v>
-      </c>
-      <c r="F22" s="8">
-        <v>2</v>
-      </c>
-      <c r="G22" s="8" t="s">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
         <v>80</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22">
         <v>4</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" t="s">
         <v>85</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" t="s">
         <v>86</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22">
         <v>6</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="8">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8">
-        <v>1</v>
-      </c>
-      <c r="F23" s="8">
-        <v>2</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23">
         <v>5</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" t="s">
         <v>88</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23">
         <v>6</v>
       </c>
-      <c r="M23" s="8" t="s">
+      <c r="M23" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="8">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="8">
-        <v>0</v>
-      </c>
-      <c r="E24" s="8">
-        <v>1</v>
-      </c>
-      <c r="F24" s="8">
-        <v>2</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24">
         <v>6</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" t="s">
         <v>91</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" t="s">
         <v>88</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24">
         <v>6</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="8">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="8">
-        <v>0</v>
-      </c>
-      <c r="E25" s="8">
-        <v>1</v>
-      </c>
-      <c r="F25" s="8">
-        <v>2</v>
-      </c>
-      <c r="G25" s="8" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
         <v>80</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" t="s">
         <v>86</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" t="s">
         <v>89</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25">
         <v>6</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="8">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26">
         <v>25</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="8">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
-        <v>2</v>
-      </c>
-      <c r="G26" s="8" t="s">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26">
         <v>7</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" t="s">
         <v>94</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" t="s">
         <v>95</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26">
         <v>6</v>
       </c>
-      <c r="M26" s="8" t="s">
+      <c r="M26" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="8">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="8">
-        <v>0</v>
-      </c>
-      <c r="E27" s="8">
-        <v>1</v>
-      </c>
-      <c r="F27" s="8">
-        <v>2</v>
-      </c>
-      <c r="G27" s="8" t="s">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
         <v>80</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" t="s">
         <v>97</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27">
         <v>6</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="8">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28">
         <v>27</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="8">
-        <v>0</v>
-      </c>
-      <c r="E28" s="8">
-        <v>1</v>
-      </c>
-      <c r="F28" s="8">
-        <v>2</v>
-      </c>
-      <c r="G28" s="8" t="s">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
         <v>80</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" t="s">
         <v>88</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28">
         <v>6</v>
       </c>
-      <c r="M28" s="8" t="s">
+      <c r="M28" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="8">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="8">
-        <v>0</v>
-      </c>
-      <c r="E29" s="8">
-        <v>1</v>
-      </c>
-      <c r="F29" s="8">
-        <v>2</v>
-      </c>
-      <c r="G29" s="8" t="s">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
         <v>80</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" t="s">
         <v>88</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29">
         <v>6</v>
       </c>
-      <c r="M29" s="8" t="s">
+      <c r="M29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="8">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30">
         <v>29</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="8">
-        <v>0</v>
-      </c>
-      <c r="E30" s="8">
-        <v>1</v>
-      </c>
-      <c r="F30" s="8">
-        <v>2</v>
-      </c>
-      <c r="G30" s="8" t="s">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
         <v>80</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="J30" t="s">
         <v>88</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30">
         <v>6</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="M30" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="8">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31">
         <v>30</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="8">
-        <v>0</v>
-      </c>
-      <c r="E31" s="8">
-        <v>1</v>
-      </c>
-      <c r="F31" s="8">
-        <v>2</v>
-      </c>
-      <c r="G31" s="8" t="s">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
         <v>80</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="J31" t="s">
         <v>88</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31">
         <v>6</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="M31" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="8">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32">
         <v>31</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="8">
-        <v>0</v>
-      </c>
-      <c r="E32" s="8">
-        <v>1</v>
-      </c>
-      <c r="F32" s="8">
-        <v>2</v>
-      </c>
-      <c r="G32" s="8" t="s">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
         <v>80</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" t="s">
         <v>88</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32">
         <v>6</v>
       </c>
-      <c r="M32" s="8" t="s">
+      <c r="M32" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="8">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33">
         <v>32</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="8">
-        <v>0</v>
-      </c>
-      <c r="E33" s="8">
-        <v>1</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>3</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" t="s">
         <v>104</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" t="s">
         <v>105</v>
       </c>
-      <c r="K33" s="8" t="s">
+      <c r="K33" t="s">
         <v>106</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33">
         <v>11</v>
       </c>
-      <c r="M33" s="8" t="s">
+      <c r="M33" t="s">
         <v>107</v>
       </c>
-      <c r="N33" s="8" t="s">
+      <c r="N33" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="8">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34">
         <v>33</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="8">
-        <v>0</v>
-      </c>
-      <c r="E34" s="8">
-        <v>1</v>
-      </c>
-      <c r="F34" s="8">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>3</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" t="s">
         <v>104</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34">
         <v>3</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I34" t="s">
         <v>110</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" t="s">
         <v>111</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K34" t="s">
         <v>112</v>
       </c>
-      <c r="L34" s="9" t="s">
+      <c r="L34" t="s">
         <v>113</v>
       </c>
-      <c r="M34" s="8" t="s">
+      <c r="M34" t="s">
         <v>114</v>
       </c>
-      <c r="N34" s="8" t="s">
+      <c r="N34" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="8">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35">
         <v>34</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="8">
-        <v>0</v>
-      </c>
-      <c r="E35" s="8">
-        <v>1</v>
-      </c>
-      <c r="F35" s="8">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>3</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" t="s">
         <v>104</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" t="s">
         <v>111</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K35" t="s">
         <v>117</v>
       </c>
-      <c r="L35" s="9" t="s">
+      <c r="L35" t="s">
         <v>118</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M35" t="s">
         <v>119</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N35" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="8">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36">
         <v>35</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="8">
-        <v>0</v>
-      </c>
-      <c r="E36" s="8">
-        <v>1</v>
-      </c>
-      <c r="F36" s="8">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>3</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" t="s">
         <v>104</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="J36" t="s">
         <v>111</v>
       </c>
-      <c r="K36" s="8" t="s">
+      <c r="K36" t="s">
         <v>122</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36">
         <v>9</v>
       </c>
-      <c r="M36" s="8" t="s">
+      <c r="M36" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="8">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37">
         <v>36</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" t="s">
         <v>124</v>
       </c>
-      <c r="D37" s="8">
-        <v>0</v>
-      </c>
-      <c r="E37" s="8">
-        <v>1</v>
-      </c>
-      <c r="F37" s="8">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>3</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" t="s">
         <v>104</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="J37" t="s">
         <v>111</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K37" t="s">
         <v>117</v>
       </c>
-      <c r="L37" s="9">
+      <c r="L37">
         <v>9</v>
       </c>
-      <c r="M37" s="8" t="s">
+      <c r="M37" t="s">
         <v>123</v>
       </c>
-      <c r="N37" s="8" t="s">
+      <c r="N37" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="8">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38">
         <v>37</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" t="s">
         <v>126</v>
       </c>
-      <c r="D38" s="8">
-        <v>0</v>
-      </c>
-      <c r="E38" s="8">
-        <v>1</v>
-      </c>
-      <c r="F38" s="8">
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
         <v>3</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" t="s">
         <v>104</v>
       </c>
-      <c r="J38" s="8" t="s">
+      <c r="J38" t="s">
         <v>127</v>
       </c>
-      <c r="L38" s="9">
+      <c r="L38">
         <v>13</v>
       </c>
-      <c r="M38" s="8" t="s">
+      <c r="M38" t="s">
         <v>128</v>
       </c>
-      <c r="N38" s="8" t="s">
+      <c r="N38" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="8">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39">
         <v>38</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="8">
-        <v>0</v>
-      </c>
-      <c r="E39" s="8">
-        <v>1</v>
-      </c>
-      <c r="F39" s="8">
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
         <v>3</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" t="s">
         <v>104</v>
       </c>
-      <c r="J39" s="8" t="s">
+      <c r="J39" t="s">
         <v>105</v>
       </c>
-      <c r="L39" s="9">
+      <c r="L39">
         <v>13</v>
       </c>
-      <c r="M39" s="8" t="s">
+      <c r="M39" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="8">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40">
         <v>39</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="8">
-        <v>0</v>
-      </c>
-      <c r="E40" s="8">
-        <v>1</v>
-      </c>
-      <c r="F40" s="8">
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
         <v>3</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="G40" t="s">
         <v>104</v>
       </c>
-      <c r="J40" s="8" t="s">
+      <c r="J40" t="s">
         <v>132</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="K40" t="s">
         <v>133</v>
       </c>
-      <c r="L40" s="9">
+      <c r="L40">
         <v>7</v>
       </c>
-      <c r="M40" s="8" t="s">
+      <c r="M40" t="s">
         <v>134</v>
       </c>
-      <c r="N40" s="8" t="s">
+      <c r="N40" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="8">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41">
         <v>40</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="8">
-        <v>0</v>
-      </c>
-      <c r="E41" s="8">
-        <v>1</v>
-      </c>
-      <c r="F41" s="8">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
         <v>3</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G41" t="s">
         <v>104</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="J41" t="s">
         <v>132</v>
       </c>
-      <c r="K41" s="8" t="s">
+      <c r="K41" t="s">
         <v>137</v>
       </c>
-      <c r="L41" s="9">
+      <c r="L41">
         <v>13</v>
       </c>
-      <c r="M41" s="8" t="s">
+      <c r="M41" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="8">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42">
         <v>41</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="8">
-        <v>0</v>
-      </c>
-      <c r="E42" s="8">
-        <v>1</v>
-      </c>
-      <c r="F42" s="8">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
         <v>3</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" t="s">
         <v>104</v>
       </c>
-      <c r="H42" s="8">
-        <v>1</v>
-      </c>
-      <c r="I42" s="1" t="s">
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
         <v>138</v>
       </c>
-      <c r="J42" s="8" t="s">
+      <c r="J42" t="s">
         <v>105</v>
       </c>
-      <c r="L42" s="9">
+      <c r="L42">
         <v>11</v>
       </c>
-      <c r="M42" s="8" t="s">
+      <c r="M42" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="8">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43">
         <v>42</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="8">
-        <v>0</v>
-      </c>
-      <c r="E43" s="8">
-        <v>2</v>
-      </c>
-      <c r="F43" s="8">
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
         <v>3</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" t="s">
         <v>104</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="J43" t="s">
         <v>105</v>
       </c>
-      <c r="L43" s="9">
+      <c r="L43">
         <v>13</v>
       </c>
-      <c r="M43" s="8" t="s">
+      <c r="M43" t="s">
         <v>128</v>
       </c>
-      <c r="N43" s="8" t="s">
+      <c r="N43" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="8">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44">
         <v>43</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" t="s">
         <v>141</v>
       </c>
-      <c r="D44" s="8">
-        <v>0</v>
-      </c>
-      <c r="E44" s="8">
-        <v>1</v>
-      </c>
-      <c r="F44" s="8">
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
         <v>4</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" t="s">
         <v>142</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" t="s">
         <v>143</v>
       </c>
-      <c r="L44" s="9">
+      <c r="L44">
         <v>3</v>
       </c>
-      <c r="M44" s="8" t="s">
+      <c r="M44" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="8">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45">
         <v>44</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="8">
-        <v>0</v>
-      </c>
-      <c r="E45" s="8">
-        <v>1</v>
-      </c>
-      <c r="F45" s="8">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
         <v>4</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G45" t="s">
         <v>142</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45">
         <v>11</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="I45" t="s">
         <v>146</v>
       </c>
-      <c r="J45" s="8" t="s">
+      <c r="J45" t="s">
         <v>143</v>
       </c>
-      <c r="K45" s="8" t="s">
+      <c r="K45" t="s">
         <v>89</v>
       </c>
-      <c r="L45" s="9" t="s">
+      <c r="L45" t="s">
         <v>147</v>
       </c>
-      <c r="M45" s="8" t="s">
+      <c r="M45" t="s">
         <v>148</v>
       </c>
-      <c r="N45" s="8" t="s">
+      <c r="N45" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="8">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46">
         <v>45</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" t="s">
         <v>150</v>
       </c>
-      <c r="D46" s="8">
-        <v>0</v>
-      </c>
-      <c r="E46" s="8">
-        <v>1</v>
-      </c>
-      <c r="F46" s="8">
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
         <v>4</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G46" t="s">
         <v>142</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="J46" t="s">
         <v>151</v>
       </c>
-      <c r="L46" s="9">
-        <v>2</v>
-      </c>
-      <c r="M46" s="8" t="s">
+      <c r="L46">
+        <v>2</v>
+      </c>
+      <c r="M46" t="s">
         <v>27</v>
       </c>
-      <c r="N46" s="8" t="s">
+      <c r="N46" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="8">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47">
         <v>46</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" t="s">
         <v>153</v>
       </c>
-      <c r="D47" s="8">
-        <v>0</v>
-      </c>
-      <c r="E47" s="8">
-        <v>2</v>
-      </c>
-      <c r="F47" s="8">
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
         <v>4</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" t="s">
         <v>142</v>
       </c>
-      <c r="J47" s="8" t="s">
+      <c r="J47" t="s">
         <v>154</v>
       </c>
-      <c r="L47" s="9">
+      <c r="L47">
         <v>10</v>
       </c>
-      <c r="M47" s="8" t="s">
+      <c r="M47" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="8">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48">
         <v>47</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" t="s">
         <v>156</v>
       </c>
-      <c r="D48" s="8">
-        <v>0</v>
-      </c>
-      <c r="E48" s="8">
-        <v>2</v>
-      </c>
-      <c r="F48" s="8">
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
         <v>4</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" t="s">
         <v>142</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="J48" t="s">
         <v>154</v>
       </c>
-      <c r="L48" s="9">
+      <c r="L48">
         <v>10</v>
       </c>
-      <c r="M48" s="8" t="s">
+      <c r="M48" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="8">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49">
         <v>48</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" t="s">
         <v>157</v>
       </c>
-      <c r="D49" s="8">
-        <v>0</v>
-      </c>
-      <c r="E49" s="8">
-        <v>2</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
         <v>5</v>
       </c>
-      <c r="G49" s="8" t="s">
+      <c r="G49" t="s">
         <v>158</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="J49" t="s">
         <v>159</v>
       </c>
-      <c r="L49" s="9" t="s">
+      <c r="L49" t="s">
         <v>160</v>
       </c>
-      <c r="M49" s="8" t="s">
+      <c r="M49" t="s">
         <v>161</v>
       </c>
-      <c r="N49" s="8" t="s">
+      <c r="N49" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="8">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50">
         <v>49</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="8">
-        <v>0</v>
-      </c>
-      <c r="E50" s="8">
-        <v>2</v>
-      </c>
-      <c r="F50" s="8">
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
         <v>5</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" t="s">
         <v>158</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="J50" t="s">
         <v>159</v>
       </c>
-      <c r="L50" s="9" t="s">
+      <c r="L50" t="s">
         <v>160</v>
       </c>
-      <c r="M50" s="8" t="s">
+      <c r="M50" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="8">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51">
         <v>50</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="8">
-        <v>0</v>
-      </c>
-      <c r="E51" s="8">
-        <v>2</v>
-      </c>
-      <c r="F51" s="8">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
         <v>5</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" t="s">
         <v>158</v>
       </c>
-      <c r="J51" s="8" t="s">
+      <c r="J51" t="s">
         <v>154</v>
       </c>
-      <c r="L51" s="9">
+      <c r="L51">
         <v>9</v>
       </c>
-      <c r="M51" s="8" t="s">
+      <c r="M51" t="s">
         <v>123</v>
       </c>
-      <c r="N51" s="8" t="s">
+      <c r="N51" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="8">
+      <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52">
         <v>51</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" t="s">
         <v>166</v>
       </c>
-      <c r="D52" s="8">
-        <v>0</v>
-      </c>
-      <c r="E52" s="8">
-        <v>2</v>
-      </c>
-      <c r="F52" s="8">
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
         <v>5</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" t="s">
         <v>158</v>
       </c>
-      <c r="J52" s="8" t="s">
+      <c r="J52" t="s">
         <v>167</v>
       </c>
-      <c r="L52" s="9">
+      <c r="L52">
         <v>9</v>
       </c>
-      <c r="M52" s="8" t="s">
+      <c r="M52" t="s">
         <v>123</v>
       </c>
-      <c r="N52" s="8" t="s">
+      <c r="N52" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="8">
+      <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53">
         <v>52</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" t="s">
         <v>169</v>
       </c>
-      <c r="D53" s="8">
-        <v>0</v>
-      </c>
-      <c r="E53" s="8">
-        <v>1</v>
-      </c>
-      <c r="F53" s="8">
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
         <v>5</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" t="s">
         <v>158</v>
       </c>
-      <c r="H53" s="8">
-        <v>2</v>
-      </c>
-      <c r="I53" s="1" t="s">
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53" t="s">
         <v>170</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="J53" t="s">
         <v>167</v>
       </c>
-      <c r="K53" s="8" t="s">
+      <c r="K53" t="s">
         <v>122</v>
       </c>
-      <c r="L53" s="9">
+      <c r="L53">
         <v>11</v>
       </c>
-      <c r="M53" s="8" t="s">
+      <c r="M53" t="s">
         <v>107</v>
       </c>
-      <c r="N53" s="8" t="s">
+      <c r="N53" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="8">
+      <c r="A54">
         <v>54</v>
       </c>
-      <c r="B54" s="8">
-        <v>1</v>
-      </c>
-      <c r="C54" s="8" t="s">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
         <v>172</v>
       </c>
-      <c r="D54" s="8">
-        <v>1</v>
-      </c>
-      <c r="E54" s="8">
-        <v>1</v>
-      </c>
-      <c r="F54" s="8">
-        <v>1</v>
-      </c>
-      <c r="G54" s="8" t="s">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
         <v>16</v>
       </c>
-      <c r="J54" s="8" t="s">
+      <c r="J54" t="s">
         <v>61</v>
       </c>
-      <c r="L54" s="9">
-        <v>2</v>
-      </c>
-      <c r="M54" s="8" t="s">
+      <c r="L54">
+        <v>2</v>
+      </c>
+      <c r="M54" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="8">
+      <c r="A55">
         <v>55</v>
       </c>
-      <c r="B55" s="8">
-        <v>2</v>
-      </c>
-      <c r="C55" s="8" t="s">
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
         <v>173</v>
       </c>
-      <c r="D55" s="8">
-        <v>1</v>
-      </c>
-      <c r="E55" s="8">
-        <v>1</v>
-      </c>
-      <c r="F55" s="8">
-        <v>1</v>
-      </c>
-      <c r="G55" s="8" t="s">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
         <v>16</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="J55" t="s">
         <v>174</v>
       </c>
-      <c r="L55" s="9">
-        <v>2</v>
-      </c>
-      <c r="M55" s="8" t="s">
+      <c r="L55">
+        <v>2</v>
+      </c>
+      <c r="M55" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="8">
+      <c r="A56">
         <v>56</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56">
         <v>3</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" t="s">
         <v>175</v>
       </c>
-      <c r="D56" s="8">
-        <v>1</v>
-      </c>
-      <c r="E56" s="8">
-        <v>1</v>
-      </c>
-      <c r="F56" s="8">
-        <v>1</v>
-      </c>
-      <c r="G56" s="8" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
         <v>16</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H56">
         <v>12</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="I56" t="s">
         <v>176</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="J56" t="s">
         <v>177</v>
       </c>
-      <c r="L56" s="9" t="s">
+      <c r="L56" t="s">
         <v>178</v>
       </c>
-      <c r="M56" s="8" t="s">
+      <c r="M56" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="1">
+      <c r="A57">
         <v>57</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57">
         <v>4</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" t="s">
         <v>180</v>
       </c>
-      <c r="D57" s="8">
-        <v>1</v>
-      </c>
-      <c r="E57" s="8">
-        <v>1</v>
-      </c>
-      <c r="F57" s="8">
-        <v>1</v>
-      </c>
-      <c r="G57" s="8" t="s">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57" t="s">
         <v>16</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="J57" t="s">
         <v>177</v>
       </c>
-      <c r="L57" s="9" t="s">
+      <c r="L57" t="s">
         <v>178</v>
       </c>
-      <c r="M57" s="8" t="s">
+      <c r="M57" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="1">
+      <c r="A58">
         <v>58</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58">
         <v>5</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" t="s">
         <v>181</v>
       </c>
-      <c r="D58" s="8">
-        <v>1</v>
-      </c>
-      <c r="E58" s="8">
-        <v>1</v>
-      </c>
-      <c r="F58" s="8">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
         <v>4</v>
       </c>
-      <c r="G58" s="8" t="s">
+      <c r="G58" t="s">
         <v>142</v>
       </c>
-      <c r="J58" s="8" t="s">
+      <c r="J58" t="s">
         <v>143</v>
       </c>
-      <c r="L58" s="9">
+      <c r="L58">
         <v>3</v>
       </c>
-      <c r="M58" s="8" t="s">
+      <c r="M58" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="1">
+      <c r="A59">
         <v>59</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59">
         <v>6</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" t="s">
         <v>182</v>
       </c>
-      <c r="D59" s="8">
-        <v>1</v>
-      </c>
-      <c r="E59" s="8">
-        <v>1</v>
-      </c>
-      <c r="F59" s="8">
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
         <v>4</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G59" t="s">
         <v>142</v>
       </c>
-      <c r="J59" s="8" t="s">
+      <c r="J59" t="s">
         <v>143</v>
       </c>
-      <c r="L59" s="9">
+      <c r="L59">
         <v>3</v>
       </c>
-      <c r="M59" s="8" t="s">
+      <c r="M59" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="1">
+      <c r="A60">
         <v>60</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60">
         <v>7</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" t="s">
         <v>183</v>
       </c>
-      <c r="D60" s="8">
-        <v>1</v>
-      </c>
-      <c r="E60" s="8">
-        <v>2</v>
-      </c>
-      <c r="F60" s="8">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
         <v>4</v>
       </c>
-      <c r="G60" s="8" t="s">
+      <c r="G60" t="s">
         <v>142</v>
       </c>
-      <c r="L60" s="9">
+      <c r="L60">
         <v>14</v>
       </c>
-      <c r="M60" s="8" t="s">
+      <c r="M60" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="1">
+      <c r="A61">
         <v>61</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61">
         <v>8</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" t="s">
         <v>184</v>
       </c>
-      <c r="D61" s="8">
-        <v>1</v>
-      </c>
-      <c r="E61" s="8">
-        <v>1</v>
-      </c>
-      <c r="F61" s="8">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
         <v>5</v>
       </c>
-      <c r="G61" s="8" t="s">
+      <c r="G61" t="s">
         <v>158</v>
       </c>
-      <c r="J61" s="8" t="s">
+      <c r="J61" t="s">
         <v>185</v>
       </c>
-      <c r="L61" s="9">
+      <c r="L61">
         <v>15</v>
       </c>
-      <c r="M61" s="8" t="s">
+      <c r="M61" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="1">
+      <c r="A62">
         <v>62</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62">
         <v>9</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" t="s">
         <v>187</v>
       </c>
-      <c r="D62" s="8">
-        <v>1</v>
-      </c>
-      <c r="E62" s="8">
-        <v>1</v>
-      </c>
-      <c r="F62" s="8">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
         <v>5</v>
       </c>
-      <c r="G62" s="8" t="s">
+      <c r="G62" t="s">
         <v>158</v>
       </c>
-      <c r="J62" s="8" t="s">
+      <c r="J62" t="s">
         <v>188</v>
       </c>
-      <c r="L62" s="9">
+      <c r="L62">
         <v>15</v>
       </c>
-      <c r="M62" s="8" t="s">
+      <c r="M62" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="1">
+      <c r="A63">
         <v>63</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B63">
         <v>10</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" t="s">
         <v>189</v>
       </c>
-      <c r="D63" s="8">
-        <v>1</v>
-      </c>
-      <c r="E63" s="8">
-        <v>1</v>
-      </c>
-      <c r="F63" s="8">
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
         <v>5</v>
       </c>
-      <c r="G63" s="8" t="s">
+      <c r="G63" t="s">
         <v>158</v>
       </c>
-      <c r="J63" s="8" t="s">
+      <c r="J63" t="s">
         <v>190</v>
       </c>
-      <c r="L63" s="9" t="s">
+      <c r="L63" t="s">
         <v>191</v>
       </c>
-      <c r="M63" s="8" t="s">
+      <c r="M63" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="1">
+      <c r="A64">
         <v>64</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64">
         <v>11</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" t="s">
         <v>193</v>
       </c>
-      <c r="D64" s="8">
-        <v>1</v>
-      </c>
-      <c r="E64" s="8">
-        <v>1</v>
-      </c>
-      <c r="F64" s="8">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
         <v>5</v>
       </c>
-      <c r="G64" s="8" t="s">
+      <c r="G64" t="s">
         <v>158</v>
       </c>
-      <c r="J64" s="8" t="s">
+      <c r="J64" t="s">
         <v>194</v>
       </c>
-      <c r="L64" s="9">
+      <c r="L64">
         <v>14</v>
       </c>
-      <c r="M64" s="8" t="s">
+      <c r="M64" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O64" xr:uid="{B1C6342A-C2BE-468B-8BFE-EEDBDB16F2F5}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O64">
-      <sortCondition ref="A2"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;A</oddHeader>
-    <oddFooter>Page &amp;P</oddFooter>
-  </headerFooter>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
 </file>
 

</xml_diff>